<commit_message>
medgulf nextcare rates update
</commit_message>
<xml_diff>
--- a/Input/Medgulf_Nextcare/benefits1.xlsx
+++ b/Input/Medgulf_Nextcare/benefits1.xlsx
@@ -292,13 +292,13 @@
     <t xml:space="preserve">Yes</t>
   </si>
   <si>
-    <t xml:space="preserve">Consultations AED 50, medicines nil co-pay/NIL</t>
+    <t xml:space="preserve">Consultations AED 50, OP NIL co-pay, Pharma NIL co-pay/NIL</t>
   </si>
   <si>
     <t xml:space="preserve">medgulf_nextcare</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-08-25</t>
+    <t xml:space="preserve">2024-10-31</t>
   </si>
   <si>
     <t xml:space="preserve">UAE - Abu Dhabi</t>
@@ -325,7 +325,7 @@
     <t xml:space="preserve">Covered up to AED 2,000 </t>
   </si>
   <si>
-    <t xml:space="preserve">Consultations AED 50, medicines 15% co-pay/15%</t>
+    <t xml:space="preserve">Consultations AED 50, OP NIL co-pay, Pharma 15% co-pay/15%</t>
   </si>
   <si>
     <t xml:space="preserve">Plan 3</t>
@@ -355,7 +355,7 @@
     <t xml:space="preserve">IP Psychiatric treatment covered up to AED 6,000/ OP Psychiatric treatment covered up to AED 1,500</t>
   </si>
   <si>
-    <t xml:space="preserve">Consultations AED 50, medicines 20% co-pay/20%</t>
+    <t xml:space="preserve">Consultations AED 50, OP NIL co-pay, Pharma 20% co-pay/20%</t>
   </si>
   <si>
     <t xml:space="preserve">Plan 4</t>
@@ -544,12 +544,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -615,40 +615,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:BJ7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BF1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BG3" activeCellId="0" sqref="BG3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="11.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="62.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="58.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="10" style="0" width="11.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="40.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="48.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="121.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="11.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="40.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="11.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="27.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="11.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="23" style="0" width="11.69"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="11.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="0" width="13.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="0" width="91.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="0" width="22.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="2" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="61" style="0" width="11.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -827,7 +820,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>58</v>
       </c>
@@ -982,7 +975,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>95</v>
       </c>
@@ -1122,7 +1115,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="34.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>102</v>
       </c>

</xml_diff>